<commit_message>
adding 4th edition edited list of tumor
</commit_message>
<xml_diff>
--- a/data/WHO_Tumors/intermediate/df_3rd_edition_manual_edit.xlsx
+++ b/data/WHO_Tumors/intermediate/df_3rd_edition_manual_edit.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lahiria/Desktop/MTP_Paper/CT-Embedding-Paper/data/WHO_Tumors/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4A20BE-03C2-7040-B1A1-DDC84E58644B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990DF59C-4520-214E-A712-4776A68DDCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3120" windowWidth="38400" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="20120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generated" sheetId="1" r:id="rId1"/>
     <sheet name="Edit_area" sheetId="3" r:id="rId2"/>
-    <sheet name="Final_List" sheetId="2" r:id="rId3"/>
+    <sheet name="Edited_Tumors" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -4095,21 +4095,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -4411,7 +4397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1135" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+    <sheetView topLeftCell="A1135" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
       <selection activeCell="D1181" sqref="D1181"/>
     </sheetView>
   </sheetViews>
@@ -20759,19 +20745,9 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Yes">
+  <conditionalFormatting sqref="B1:D1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",B1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22646,7 +22622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0C7095-BB2C-B645-B6DC-8C51C2B6F00C}">
   <dimension ref="A1:A1535"/>
   <sheetViews>
-    <sheetView topLeftCell="A226" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
       <selection activeCell="C372" sqref="C372"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates to 5th, 4th, 3rd edition for radial scars
</commit_message>
<xml_diff>
--- a/data/WHO_Tumors/intermediate/df_3rd_edition_manual_edit.xlsx
+++ b/data/WHO_Tumors/intermediate/df_3rd_edition_manual_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lahiria/Desktop/MTP_Paper/CT-Embedding-Paper/data/WHO_Tumors/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990DF59C-4520-214E-A712-4776A68DDCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17324F4-EAA0-5049-8439-60CFC119D79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="20120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3120" windowWidth="38400" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generated" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6572" uniqueCount="1344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6572" uniqueCount="1345">
   <si>
     <t>Tumor_Names</t>
   </si>
@@ -4054,6 +4054,9 @@
   </si>
   <si>
     <t>mpnst with divergent epithelial differentiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">radial scar </t>
   </si>
 </sst>
 </file>
@@ -22622,8 +22625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0C7095-BB2C-B645-B6DC-8C51C2B6F00C}">
   <dimension ref="A1:A1535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
-      <selection activeCell="C372" sqref="C372"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23033,7 +23036,7 @@
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>1207</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update till 438 5th edition
</commit_message>
<xml_diff>
--- a/data/WHO_Tumors/intermediate/df_3rd_edition_manual_edit.xlsx
+++ b/data/WHO_Tumors/intermediate/df_3rd_edition_manual_edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lahiria/Desktop/MTP_Paper/CT-Embedding-Paper/data/WHO_Tumors/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17324F4-EAA0-5049-8439-60CFC119D79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB00F643-E456-EB44-92DA-2A80B307E72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3120" windowWidth="38400" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6572" uniqueCount="1345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6572" uniqueCount="1346">
   <si>
     <t>Tumor_Names</t>
   </si>
@@ -4057,6 +4057,9 @@
   </si>
   <si>
     <t xml:space="preserve">radial scar </t>
+  </si>
+  <si>
+    <t>myositis ossificans</t>
   </si>
 </sst>
 </file>
@@ -22625,8 +22628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0C7095-BB2C-B645-B6DC-8C51C2B6F00C}">
   <dimension ref="A1:A1535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23991,7 +23994,7 @@
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>1302</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>